<commit_message>
Grow Constraint Upwards Proposal + remove duplicates
</commit_message>
<xml_diff>
--- a/Experiments.xlsx
+++ b/Experiments.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/meghanachilukuri/bayou_mcmc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BF9ADEC-F815-F347-809C-B1ABF8AAF755}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD1FE2AC-46C9-B24F-BC51-C7B48A2C12BB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{3E4EDB3B-C1A3-824E-B263-86E2B3584FEB}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="31">
   <si>
     <t>Single API</t>
   </si>
@@ -111,13 +111,22 @@
     <t>Accuracy Test - Pairs</t>
   </si>
   <si>
-    <t>Notes: In the bayou paper, they do it based on whether the expected program is in the top 10 results or not.   Should I have max length?                           May nee to have Inclusion/Exclusion of control structures differently</t>
-  </si>
-  <si>
     <t>Include APIs</t>
   </si>
   <si>
     <t>Exclude APIs</t>
+  </si>
+  <si>
+    <t>User studies</t>
+  </si>
+  <si>
+    <t>Examples to show:</t>
+  </si>
+  <si>
+    <t>Notes: In the bayou paper, they do it based on whether the expected program is in the top 10 results or not.   Should I have max length?                           May need to have Inclusion/Exclusion of control structures differently - yes</t>
+  </si>
+  <si>
+    <t>bayou-vae-mcmc side by side</t>
   </si>
 </sst>
 </file>
@@ -738,8 +747,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F95F159A-0EF3-DE4D-BEED-B69B79CB6154}">
   <dimension ref="A1:L63"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2"/>
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -773,7 +782,7 @@
       <c r="G1" s="5"/>
       <c r="H1" s="6"/>
       <c r="J1" s="17" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="K1" s="17"/>
       <c r="L1" s="17"/>
@@ -812,7 +821,7 @@
     </row>
     <row r="4" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A4" s="19" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B4" s="32" t="s">
         <v>0</v>
@@ -908,7 +917,7 @@
     </row>
     <row r="11" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A11" s="19" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B11" s="32" t="s">
         <v>0</v>
@@ -1572,14 +1581,32 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5D018F6-1E6C-3741-9230-CC2D98087BE3}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="26.1640625" customWidth="1"/>
+    <col min="2" max="2" width="24.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>